<commit_message>
perbaikan dan tambah banyak fitur
</commit_message>
<xml_diff>
--- a/uploads/import/format/soal.xlsx
+++ b/uploads/import/format/soal.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WEB_APP\ALIAS_WWW\oltest\uploads\import\format\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WEB_APP\ALIAS_WWW\ujianundip\uploads\import\format\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7150024F-F096-4FC9-B8F3-1831F2BB6E64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{938EC663-94F5-4EAB-AFC5-8A18C5B24E0E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>TOPIK ID</t>
   </si>
@@ -49,6 +49,15 @@
   </si>
   <si>
     <t>OPSI E</t>
+  </si>
+  <si>
+    <t>GEL</t>
+  </si>
+  <si>
+    <t>SMT</t>
+  </si>
+  <si>
+    <t>TAHUN</t>
   </si>
 </sst>
 </file>
@@ -404,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -420,7 +429,7 @@
     <col min="10" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:12">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -447,6 +456,15 @@
       </c>
       <c r="I1" s="3" t="s">
         <v>7</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
perbaikan mayor untuk controller auth
</commit_message>
<xml_diff>
--- a/uploads/import/format/soal.xlsx
+++ b/uploads/import/format/soal.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WEB_APP\ALIAS_WWW\ujianundip\uploads\import\format\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{938EC663-94F5-4EAB-AFC5-8A18C5B24E0E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{950C5B8C-B3F8-4ABC-9E48-536FB4489146}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>TOPIK ID</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>TAHUN</t>
+  </si>
+  <si>
+    <t>PENJELASAN</t>
   </si>
 </sst>
 </file>
@@ -413,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -424,12 +427,12 @@
     <col min="1" max="1" width="15.75" style="3" customWidth="1"/>
     <col min="2" max="2" width="55.125" style="3" customWidth="1"/>
     <col min="3" max="3" width="45.625" style="4" customWidth="1"/>
-    <col min="4" max="8" width="36.625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="32.75" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="9" style="2"/>
+    <col min="4" max="9" width="36.625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="32.75" style="3" customWidth="1"/>
+    <col min="11" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -455,15 +458,18 @@
         <v>6</v>
       </c>
       <c r="I1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>